<commit_message>
Coempt updates based on projects with Gita
</commit_message>
<xml_diff>
--- a/target/test-classes/Test_datas/SCTE_VT/Book1.xlsx
+++ b/target/test-classes/Test_datas/SCTE_VT/Book1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>ID</t>
   </si>
@@ -52,25 +52,13 @@
   </si>
   <si>
     <t>Advance Manufacturing Processes</t>
-  </si>
-  <si>
-    <t>student registration number</t>
-  </si>
-  <si>
-    <t>Semester</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>Sem Mark</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,11 +71,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -110,11 +93,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,10 +412,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A2:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,20 +426,6 @@
     <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>

</xml_diff>